<commit_message>
change scheduling and correct get job type in linkedin module
</commit_message>
<xml_diff>
--- a/static/main_cryptocurrency.xlsx
+++ b/static/main_cryptocurrency.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A58"/>
+  <dimension ref="A1:A72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -835,7 +835,105 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>https://cryptocurrencyjobs.co/marketing/foundation-senior-copywriter-contract/</t>
+          <t>https://cryptocurrencyjobs.co/operations/futuremoney-group-operation-events-coordinator/</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>https://cryptocurrencyjobs.co/engineering/chainlink-incident-responder-apac/</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>https://cryptocurrencyjobs.co/marketing/chainlink-market-strategy-manager-capital-markets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>https://cryptocurrencyjobs.co/engineering/chainlink-principal-engineer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>https://cryptocurrencyjobs.co/engineering/chainlink-research-engineer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>https://cryptocurrencyjobs.co/sales/chainlink-senior-data-partnerships-manager/</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>https://cryptocurrencyjobs.co/engineering/chainlink-senior-site-reliability-engineer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>https://cryptocurrencyjobs.co/operations/chainlink-strategic-finance-manager/</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>https://cryptocurrencyjobs.co/engineering/chainlink-engineering-manager-blockchain-integrations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>https://cryptocurrencyjobs.co/sales/chainlink-technical-account-manager/</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>https://cryptocurrencyjobs.co/engineering/ontropy-senior-blockchain-engineer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>https://cryptocurrencyjobs.co/sales/gelato-network-business-development-internship/</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>https://cryptocurrencyjobs.co/operations/chainlink-senior-people-business-partner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>https://cryptocurrencyjobs.co/marketing/gridplus-marketing-director/</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>https://cryptocurrencyjobs.co/marketing/blockdaemon-growth-strategy-lead/</t>
         </is>
       </c>
     </row>

</xml_diff>